<commit_message>
InitialUI renamed, new data, pandas ver removed
</commit_message>
<xml_diff>
--- a/data/output_data.xlsx
+++ b/data/output_data.xlsx
@@ -8,6 +8,8 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -588,4 +590,534 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Кількість елементів</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Середній час</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Кількість елементів</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Точність</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>B&amp;B</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Greed</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ACO</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>B&amp;B</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Greed</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>ACO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3.100000321865082e-05</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.002045609999913722</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.08273572000180138</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3.619999915827066e-05</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.003190910002740566</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.1229132299980847</v>
+      </c>
+      <c r="F4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>7</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4.355000128271058e-05</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.01396054999931948</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1651210500000161</v>
+      </c>
+      <c r="F5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5.860000237589702e-05</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.03141236000083154</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1737159000040265</v>
+      </c>
+      <c r="F6" t="n">
+        <v>8</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>9</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6.352000054903329e-05</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.05206127000274137</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.2363194600024144</v>
+      </c>
+      <c r="F7" t="n">
+        <v>9</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>10</v>
+      </c>
+      <c r="B8" t="n">
+        <v>8.221999887609854e-05</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.6565208600033656</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.2633120999991661</v>
+      </c>
+      <c r="F8" t="n">
+        <v>10</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>11</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.0001598099988768809</v>
+      </c>
+      <c r="C9" t="n">
+        <v>7.037033379996137</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.8054246999978204</v>
+      </c>
+      <c r="F9" t="n">
+        <v>11</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>12</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.0001328599959379062</v>
+      </c>
+      <c r="C10" t="n">
+        <v>7.806809709999652</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.4187305200000992</v>
+      </c>
+      <c r="F10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>13</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.0001266500024939887</v>
+      </c>
+      <c r="C11" t="n">
+        <v>116.5706978299975</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.4791568699976779</v>
+      </c>
+      <c r="F11" t="n">
+        <v>13</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Кількість елементів</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Середній час</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Кількість елементів</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Точність</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>B&amp;B</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Greed</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ACO</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>B&amp;B</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Greed</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>ACO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3.027000639121979e-05</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.001713790002395399</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.08025141999823973</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5.331000429578126e-05</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.01992319999844767</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.1472878600063268</v>
+      </c>
+      <c r="F4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>9</v>
+      </c>
+      <c r="B5" t="n">
+        <v>7.309000066015869e-05</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1057229499972891</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.2366165999992518</v>
+      </c>
+      <c r="F5" t="n">
+        <v>9</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B6" t="n">
+        <v>9.344999853055924e-05</v>
+      </c>
+      <c r="C6" t="n">
+        <v>41.53612096000579</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.3472341199987568</v>
+      </c>
+      <c r="F6" t="n">
+        <v>11</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>13</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.0001149299961980432</v>
+      </c>
+      <c r="C7" t="n">
+        <v>108.860699790009</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.651249509997433</v>
+      </c>
+      <c r="F7" t="n">
+        <v>13</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>